<commit_message>
[Test Needed] Commemorations and Climate
</commit_message>
<xml_diff>
--- a/文档/着力点和时代.xlsx
+++ b/文档/着力点和时代.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EE5DB-D8C2-4F25-A9DE-751D0A4906D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8ED616-C9D6-47BD-9A6D-B12E58D5C36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="855" windowWidth="27915" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>百花齐放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>自由探索</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -207,7 +203,7 @@
   </si>
   <si>
     <r>
-      <t>间谍前往敌方城市不需要时间，</t>
+      <t>启发额外提供10%的市政成本。所有城市每个区域</t>
     </r>
     <r>
       <rPr>
@@ -218,13 +214,23 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>间谍进行进攻性任务的等级+4。购买间谍需要的成本-90%。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>启发额外提供10%的市政成本。所有城市每个区域</t>
+      <t>（包括市中心）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+1文化。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>异大陆城市：创建时+3人口，+2忠诚度，</t>
     </r>
     <r>
       <rPr>
@@ -235,7 +241,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>（包括市中心）</t>
+      <t>+15%粮锤</t>
     </r>
     <r>
       <rPr>
@@ -245,13 +251,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>+1文化。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>异大陆城市：创建时+3人口，+2忠诚度，</t>
+      <t>。海军和水运单位+2移动力</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>解锁一种特殊战争借口，比正式战争的战争狂惩罚低75%且可以在谴责目标后立即使用。</t>
     </r>
     <r>
       <rPr>
@@ -262,48 +268,52 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>+15%粮锤</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>。海军和水运单位+2移动力</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>解锁一种特殊战争借口，比正式战争的战争狂惩罚低75%且可以在谴责目标后立即使用。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>每个军营及其建筑提供+2生产力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>每个军营及其建筑提供+2生产力</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t>，生产军事单位+15%生产力</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>，生产军事单位+15%生产力</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+      <t>世界奇观+50%旅游业绩。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>国家公园+100%旅游业绩。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>琴棋书画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>间谍前往敌方城市不需要时间，</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -313,17 +323,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>世界奇观+50%旅游业绩。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>国家公园+100%旅游业绩。</t>
+      <t>间谍进行进攻性任务的等级+4。购买间谍需要的成本-75%。</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -405,10 +405,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13:I13"/>
     </sheetView>
   </sheetViews>
@@ -739,12 +739,12 @@
     </row>
     <row r="2" spans="1:10" ht="57" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -754,12 +754,12 @@
     </row>
     <row r="3" spans="1:10" ht="50.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -771,11 +771,11 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -784,13 +784,13 @@
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -799,67 +799,67 @@
     </row>
     <row r="6" spans="1:10" ht="55.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="55.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="55.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="55.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="55.5" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -867,44 +867,44 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="55.5" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="108" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -912,14 +912,19 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="3"/>
+      <c r="H13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D6:F6"/>
@@ -927,11 +932,6 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="H13:I13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>